<commit_message>
chore : fe/ 코드 주석 정리
</commit_message>
<xml_diff>
--- a/quality-fe/public/template.xlsx
+++ b/quality-fe/public/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MES_PROJECT\01.WebProject\Quality-Inspection\quality-fe\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34A7A24-26FB-4F6F-9947-5A0E62DF60FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DAAB40-51A0-4F67-865E-A4D71D949030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{759AA15A-92F8-448F-BFBA-D7C88A4076E8}"/>
+    <workbookView xWindow="31170" yWindow="870" windowWidth="24210" windowHeight="9915" xr2:uid="{759AA15A-92F8-448F-BFBA-D7C88A4076E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -423,10 +423,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>